<commit_message>
1. Update hero ground smash logic; 2. Critical hit ratio fixed to 1.5f; 3. GameArena updates:     (1) Scale up entire background, and zoom out main camera;     (2) Hero animation apply root;     (3) Reorganized scene architecture.
</commit_message>
<xml_diff>
--- a/Document/Workplan.xlsx
+++ b/Document/Workplan.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="3.17-3.24" sheetId="1" r:id="rId1"/>
+    <sheet name="3.25-4.1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Yangwei</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,6 +54,50 @@
   </si>
   <si>
     <t>Navigation UI document</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Forge System</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items(Heros, Weapons, Boosters, Skills) Config</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Global constants definition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Customizable Weapon And booster storage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avatar weapon replacement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item Enhancement System</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xp &amp; Coins collection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items Buy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LevelUp (Configs and logic)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avatar animation complete (start hit, gournd hit, air hit)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Floor enemy, Fly enemy design</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -404,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -466,4 +511,90 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="27.875" customWidth="1"/>
+    <col min="2" max="2" width="71.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>